<commit_message>
Pass 06/06/2022 pretty nice original solution
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan.hu\Documents\GitHub\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A03A67C3-B2E0-401E-8D30-243FA2D83F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE587ABE-0232-4E14-962F-F986377B87A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grind-169-checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -637,7 +649,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1517,26 +1529,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="2"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1560,17 +1572,17 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>202</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.37278106508875741</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>0.38461538461538464</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1591,7 +1603,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1611,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1631,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1651,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1671,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1691,7 +1703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1711,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1731,7 +1743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1751,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1771,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1791,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1811,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1831,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1851,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1871,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1891,7 +1903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1911,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1931,7 +1943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1951,7 +1963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1971,7 +1983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1991,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2011,7 +2023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2031,7 +2043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2051,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2071,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2091,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2111,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2131,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2151,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2171,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2191,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2211,7 +2223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2231,7 +2243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2251,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2268,10 +2280,10 @@
         <v>23</v>
       </c>
       <c r="F36" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2291,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2311,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2331,7 +2343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2351,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2371,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2411,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2431,7 +2443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2451,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2471,7 +2483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2491,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2511,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2531,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2551,7 +2563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2571,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2591,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2611,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2631,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2651,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2671,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2691,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2711,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2731,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2751,7 +2763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2771,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2791,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2811,7 +2823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2831,7 +2843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2851,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2871,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2891,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2911,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2931,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2948,10 +2960,10 @@
         <v>62</v>
       </c>
       <c r="F70" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2971,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2991,7 +3003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3011,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3031,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3051,7 +3063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3071,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3091,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3111,7 +3123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3131,7 +3143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3151,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3171,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3191,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3211,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3231,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3251,7 +3263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3271,7 +3283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3291,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3311,7 +3323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3331,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3351,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3371,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3391,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3411,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3431,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3451,7 +3463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3471,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3491,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3511,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3531,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3551,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3571,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3591,7 +3603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3611,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3631,7 +3643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3651,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3671,7 +3683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3691,7 +3703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3711,7 +3723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3731,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3751,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3771,7 +3783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3791,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3811,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3831,7 +3843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3851,7 +3863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3871,7 +3883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3891,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3911,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3931,7 +3943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3951,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3971,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3991,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4011,7 +4023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4031,7 +4043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4051,7 +4063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4071,7 +4083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4091,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4111,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4131,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4151,7 +4163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4171,7 +4183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4191,7 +4203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4211,7 +4223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4231,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4251,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4271,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4291,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4311,7 +4323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4331,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4351,7 +4363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4371,7 +4383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4391,7 +4403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4411,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4431,7 +4443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4451,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4471,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4491,7 +4503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4511,7 +4523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4531,7 +4543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4551,7 +4563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4571,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4591,7 +4603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4611,7 +4623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4631,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4651,7 +4663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4671,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4691,7 +4703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4711,7 +4723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4731,7 +4743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4751,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4771,7 +4783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4791,7 +4803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>162</v>
       </c>
@@ -4811,7 +4823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>163</v>
       </c>
@@ -4831,7 +4843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>164</v>
       </c>
@@ -4851,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>165</v>
       </c>
@@ -4871,7 +4883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>166</v>
       </c>
@@ -4891,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>167</v>
       </c>
@@ -4911,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>168</v>
       </c>
@@ -4931,7 +4943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
Pass 06/06/2022 #worksfirsttime slow solution
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan.hu\Documents\GitHub\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C2AF20-CD16-4BC0-846E-37B4A698B2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50CE5CF-38FB-454B-A4A1-B186AB548539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1533,8 +1533,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1572,14 +1572,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>202</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.40828402366863903</v>
+        <v>0.41420118343195267</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -2580,7 +2580,7 @@
         <v>23</v>
       </c>
       <c r="F51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Pass 08/06/2022 #worksfirsttime #solvedin10min
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B994229-0B5F-4A69-98FE-0802A68E8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CE4F2E-A955-452B-A75E-17A92E8DEA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1521,8 +1521,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,14 +1560,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>202</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.46745562130177515</v>
+        <v>0.47337278106508873</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2708,7 +2708,7 @@
         <v>19</v>
       </c>
       <c r="F58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 09/06/2022 #worksfirsttime slow one-pass with queue
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7502403B-AD7F-4279-9ADA-D9C5541CA162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE60454-0187-47F8-A927-346356A472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1521,8 +1521,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H113" sqref="H113"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,14 +1560,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>202</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.48520710059171596</v>
+        <v>0.4911242603550296</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3328,7 +3328,7 @@
         <v>14</v>
       </c>
       <c r="F89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 09/06/2022 #worksfirsttime storing iterators instead of string copies to save memory
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE60454-0187-47F8-A927-346356A472A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434E3DB6-20E7-48E3-A5CB-4BA4C090DF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1522,7 +1522,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
+      <selection pane="bottomLeft" activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,14 +1560,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>202</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.4911242603550296</v>
+        <v>0.49704142011834318</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3388,7 +3388,7 @@
         <v>34</v>
       </c>
       <c r="F92" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 09/06/2022 super slow original solution
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434E3DB6-20E7-48E3-A5CB-4BA4C090DF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4B134D-7C41-4F29-A722-00F69CF3420E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1521,8 +1521,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H92" sqref="H92"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,14 +1560,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>202</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.49704142011834318</v>
+        <v>0.50295857988165682</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3408,7 +3408,7 @@
         <v>19</v>
       </c>
       <c r="F93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 09/06/2022 bog standard solution
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6F5DF6-FA67-4E66-B9CA-404C0BB9F718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC1CCC3-1815-4F3C-8323-2543D2387A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,8 +1518,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E136" sqref="E136"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,14 +1557,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.50887573964497046</v>
+        <v>0.51479289940828399</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3905,7 +3905,7 @@
         <v>23</v>
       </c>
       <c r="F118" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 09/06/2022 slow af boi
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC1CCC3-1815-4F3C-8323-2543D2387A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1719F447-8292-43B8-BFF1-4E666EDD3FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,8 +1518,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G117" sqref="G117"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,14 +1557,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.51479289940828399</v>
+        <v>0.52071005917159763</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3485,7 +3485,7 @@
         <v>23</v>
       </c>
       <c r="F97" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 10/06/2022 don't be afraid to use bitset
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan.hu\Documents\GitHub\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1719F447-8292-43B8-BFF1-4E666EDD3FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AA999C-790C-42AA-964B-EB94B6D97B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grind-169-checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1518,22 +1530,22 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H101" sqref="H101"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="2"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1557,17 +1569,17 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.52071005917159763</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>0.53254437869822491</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1588,7 +1600,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1608,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1648,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1668,7 +1680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1688,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1708,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1728,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1748,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1768,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1788,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1808,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1828,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1848,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1868,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1888,7 +1900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1908,7 +1920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1928,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1948,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1968,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1988,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2008,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2028,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2048,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2068,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2088,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2108,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2128,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2148,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2168,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2188,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2208,7 +2220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2228,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2248,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2268,7 +2280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2288,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2308,7 +2320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2328,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2348,7 +2360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2368,7 +2380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2388,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2408,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2428,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2448,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2468,7 +2480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2508,7 +2520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2528,7 +2540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2548,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2568,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2588,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2608,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2628,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2648,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2668,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2688,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2708,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2728,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2748,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2768,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2788,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2808,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2828,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2848,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2868,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2888,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2908,7 +2920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2928,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2948,7 +2960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2968,7 +2980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2988,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3008,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3028,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3048,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3068,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3088,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3108,7 +3120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3148,7 +3160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3168,7 +3180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3188,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3208,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3228,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3248,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3268,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3288,7 +3300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3308,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3328,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3348,7 +3360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3368,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3388,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3408,7 +3420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3428,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3448,7 +3460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3468,7 +3480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3488,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3508,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3528,7 +3540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3548,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3568,7 +3580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3588,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3608,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3628,7 +3640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3648,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3668,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3688,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3708,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3728,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3748,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3768,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3788,7 +3800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3808,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3828,7 +3840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3848,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3868,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3888,7 +3900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3908,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3928,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3948,7 +3960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3968,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3988,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4008,7 +4020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4028,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4048,7 +4060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4068,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4088,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4108,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4128,7 +4140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4148,7 +4160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4168,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4188,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4208,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4228,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4248,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4268,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4288,7 +4300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4308,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4328,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4348,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4368,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4388,7 +4400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4408,7 +4420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4428,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4448,7 +4460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4468,7 +4480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4488,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4508,7 +4520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4528,7 +4540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4548,7 +4560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4568,7 +4580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4588,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4608,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4628,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4645,10 +4657,10 @@
         <v>74</v>
       </c>
       <c r="F155" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4668,7 +4680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4688,7 +4700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4708,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4728,7 +4740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4748,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4768,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4788,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>162</v>
       </c>
@@ -4808,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>163</v>
       </c>
@@ -4825,10 +4837,10 @@
         <v>9</v>
       </c>
       <c r="F164" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>164</v>
       </c>
@@ -4848,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>165</v>
       </c>
@@ -4868,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>166</v>
       </c>
@@ -4888,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>167</v>
       </c>
@@ -4908,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>168</v>
       </c>
@@ -4928,7 +4940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
Pass 12/06/2022 #worksfirsttime O(n) hint
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -1,33 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan.hu\Documents\GitHub\self-study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AA999C-790C-42AA-964B-EB94B6D97B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECAE424-C6E8-4A2C-9368-48BF86CEEE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grind-169-checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1530,22 +1518,22 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G157" sqref="G157"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="2"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" customWidth="1"/>
-    <col min="9" max="9" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1569,17 +1557,17 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.53254437869822491</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>0.53846153846153844</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1600,7 +1588,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1620,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1640,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1660,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1680,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1700,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1720,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1740,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1760,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1780,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1800,7 +1788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1820,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1840,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1860,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1880,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1900,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1920,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1940,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1960,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1980,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2000,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2020,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2040,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2060,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2080,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2100,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2120,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2140,7 +2128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2160,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2180,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2200,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2220,7 +2208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2240,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2260,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2280,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2300,7 +2288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2320,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2340,7 +2328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2360,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2380,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2400,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2420,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2440,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2457,10 +2445,10 @@
         <v>12</v>
       </c>
       <c r="F45" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2480,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2500,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2520,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2540,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2560,7 +2548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2580,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2600,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2620,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2640,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2660,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2680,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2700,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2720,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2740,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2760,7 +2748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2780,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2800,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2820,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2840,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2860,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2880,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2900,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2920,7 +2908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2940,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2960,7 +2948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2980,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3000,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3020,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3040,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3060,7 +3048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3080,7 +3068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3100,7 +3088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3120,7 +3108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3140,7 +3128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3160,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3180,7 +3168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3200,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3220,7 +3208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3240,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3260,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3280,7 +3268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3300,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3320,7 +3308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3340,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3360,7 +3348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3380,7 +3368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3400,7 +3388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3420,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3440,7 +3428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3460,7 +3448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3480,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3500,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3520,7 +3508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3540,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3560,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3580,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3600,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3620,7 +3608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3640,7 +3628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3660,7 +3648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3680,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3700,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3720,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3740,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3760,7 +3748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3780,7 +3768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3800,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3820,7 +3808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3840,7 +3828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3860,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3880,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3900,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3920,7 +3908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3940,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3960,7 +3948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3980,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4000,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4020,7 +4008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4040,7 +4028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4060,7 +4048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4080,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4100,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4120,7 +4108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4140,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4160,7 +4148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4180,7 +4168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4200,7 +4188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4220,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4240,7 +4228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4260,7 +4248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4280,7 +4268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4300,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4320,7 +4308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4340,7 +4328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4360,7 +4348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4380,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4400,7 +4388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4420,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4440,7 +4428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4460,7 +4448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4480,7 +4468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4500,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4520,7 +4508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4540,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4560,7 +4548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4580,7 +4568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4600,7 +4588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4620,7 +4608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4640,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4660,7 +4648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4680,7 +4668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4700,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4720,7 +4708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4740,7 +4728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4760,7 +4748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4780,7 +4768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4800,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -4820,7 +4808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -4840,7 +4828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -4860,7 +4848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -4880,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -4900,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -4920,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -4940,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
Pass 13/06/2022 slow af
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECAE424-C6E8-4A2C-9368-48BF86CEEE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124FE624-15B3-4FAB-BC18-8C561CFEC45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,8 +1518,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,14 +1557,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.53846153846153844</v>
+        <v>0.54437869822485208</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2665,7 +2665,7 @@
         <v>83</v>
       </c>
       <c r="F56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 13/06/2022 #worksfirsttime slow af
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124FE624-15B3-4FAB-BC18-8C561CFEC45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFE4183-CF12-4E82-8702-32B6F1C8A747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,8 +1518,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,14 +1557,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.54437869822485208</v>
+        <v>0.55029585798816572</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3085,7 +3085,7 @@
         <v>12</v>
       </c>
       <c r="F77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 13/06/2022 very fast solution
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68940A5C-65AF-4AB2-B872-E76E3AF3A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE896A5-0748-4157-AB0A-EEE60D69C7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,8 +1518,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,14 +1557,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.55621301775147924</v>
+        <v>0.56213017751479288</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3545,7 +3545,7 @@
         <v>19</v>
       </c>
       <c r="F100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 13/06/2022 #worksfirsttime DFS with move semantics
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE896A5-0748-4157-AB0A-EEE60D69C7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8760AA-75B4-4B61-A434-A2C8A990FF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,8 +1518,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H102" sqref="H102"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G139" sqref="G139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,14 +1557,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.56213017751479288</v>
+        <v>0.56804733727810652</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4205,7 +4205,7 @@
         <v>19</v>
       </c>
       <c r="F133" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 14/06/2022 Floyd's Cycle Detection Algorithm
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8760AA-75B4-4B61-A434-A2C8A990FF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0506A90B-E12C-4F66-B99B-8F6CF3E95D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="204">
   <si>
     <t>Number</t>
   </si>
@@ -629,6 +629,9 @@
   </si>
   <si>
     <t>Num Done</t>
+  </si>
+  <si>
+    <t>Floyd Cycle Detection</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1521,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G139" sqref="G139"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,14 +1560,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.56804733727810652</v>
+        <v>0.57396449704142016</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3362,10 +3365,10 @@
         <v>11</v>
       </c>
       <c r="E91" t="s">
-        <v>74</v>
+        <v>203</v>
       </c>
       <c r="F91" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 15/06/2022 so many damn concepts to incorporate
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E642AE-E6CC-46B7-BEEA-623E7798C40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A568019A-DB9F-425A-9C7F-4E276CC6277A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1525,7 +1525,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E140" sqref="E140"/>
+      <selection pane="bottomLeft" activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,14 +1563,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.57396449704142016</v>
+        <v>0.57988165680473369</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4351,7 +4351,7 @@
         <v>204</v>
       </c>
       <c r="F140" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 15/06/2022 #worksfirsttime slow af
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5FD6C5-5FA2-479A-9751-72C3D1361CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C19C9F8-62F6-45CB-ABF6-9821CEA28AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1524,8 +1524,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H156" sqref="H156"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,14 +1563,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.58579881656804733</v>
+        <v>0.59171597633136097</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4571,7 +4571,7 @@
         <v>19</v>
       </c>
       <c r="F151" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
WIP more tricky than initially thought
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C19C9F8-62F6-45CB-ABF6-9821CEA28AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1885E30C-04F7-434D-86E0-51D87FF65B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="206">
   <si>
     <t>Number</t>
   </si>
@@ -635,6 +635,9 @@
   </si>
   <si>
     <t>Kahn Topological Sort</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -1524,8 +1527,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I148" sqref="I148"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I149" sqref="I149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3670,8 +3673,8 @@
       <c r="E106" t="s">
         <v>19</v>
       </c>
-      <c r="F106" s="2">
-        <v>0</v>
+      <c r="F106" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 16/06/2022 #worksfirsttime Finally learnt Manacher's Algorithm
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1885E30C-04F7-434D-86E0-51D87FF65B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1239A013-896E-49E5-8F1C-7630071F00D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1527,8 +1527,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I149" sqref="I149"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,14 +1566,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.59171597633136097</v>
+        <v>0.59763313609467461</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
         <v>17</v>
       </c>
       <c r="F59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 28/06/2022 #worksfirsttime universal binary search algorithm
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B998F95-242F-4C1D-9F60-C77452FC50C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9FDC12-8F70-4B49-9B46-3FAF0D5FE754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="grind-169-checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1527,8 +1528,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I148" sqref="I148"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,14 +1567,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.60355029585798814</v>
+        <v>0.60946745562130178</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4294,7 +4295,7 @@
         <v>21</v>
       </c>
       <c r="F137" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pass 29/06/2022 pretty damn optimal
</commit_message>
<xml_diff>
--- a/grind-169-checklist.xlsx
+++ b/grind-169-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanh\Documents\LocalWorkCopy\self-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9FDC12-8F70-4B49-9B46-3FAF0D5FE754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA7AC2E-1C22-497D-9FEC-AD03C7835216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1528,8 +1528,8 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H139" sqref="H139"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,14 +1567,14 @@
       </c>
       <c r="H1" s="5">
         <f>COUNTIF(F2:F170, 1)</f>
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>201</v>
       </c>
       <c r="J1" s="7">
         <f>H1/169</f>
-        <v>0.60946745562130178</v>
+        <v>0.61538461538461542</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3815,7 +3815,7 @@
         <v>27</v>
       </c>
       <c r="F113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>